<commit_message>
se sube primera version de detalle de cursos
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\Documentos\documentos-6069Colegio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73F922A-E264-4000-A723-8542B9921208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD9988B5-96EC-4A50-B13D-BA59DC25242F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="148">
   <si>
     <t>Trabajo</t>
   </si>
@@ -482,9 +482,6 @@
   </si>
   <si>
     <t>Fecha de inicio 20/12/2020</t>
-  </si>
-  <si>
-    <t>Cambio</t>
   </si>
 </sst>
 </file>
@@ -716,7 +713,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -810,6 +807,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1179,9 +1179,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F832728-0D0A-4016-B1EB-6B174C9DD2A3}">
-  <dimension ref="A4:AD19"/>
+  <dimension ref="A4:AD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1385,11 +1385,6 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>148</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1400,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422FE6B-CB5A-4468-BBA6-820503F36902}">
   <dimension ref="B2:L82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1427,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1446,7 +1441,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="42" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1460,7 +1455,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="42" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1474,7 +1469,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="42" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -1516,7 +1511,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="42" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1534,7 +1529,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="42" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1638,7 +1633,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="42" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1655,7 +1650,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="42" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1666,7 +1661,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="42" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1743,7 +1738,7 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="42" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1754,7 +1749,7 @@
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="42" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1765,7 +1760,7 @@
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="42" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1776,7 +1771,7 @@
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="2" t="s">

</xml_diff>

<commit_message>
carga y descarga de archivos
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD9988B5-96EC-4A50-B13D-BA59DC25242F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C232690C-583F-42E1-AED5-6C65ECB82352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -778,6 +778,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -807,9 +810,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1396,7 +1396,7 @@
   <dimension ref="B2:L82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +1427,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="32" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1441,7 +1441,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1455,7 +1455,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="32" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="32" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -1511,7 +1511,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="32" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1529,7 +1529,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="32" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1633,7 +1633,7 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="32" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1650,7 +1650,7 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="32" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1661,7 +1661,7 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="32" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1738,7 +1738,7 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="32" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1749,7 +1749,7 @@
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="32" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1760,7 +1760,7 @@
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="32" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1771,7 +1771,7 @@
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="32" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2342,8 +2342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036ED907-70B5-4584-9CA2-BB67995731BE}">
   <dimension ref="F3:S14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,31 +2353,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="34" t="s">
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="35" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="37" t="s">
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="Q3" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="37" t="s">
+      <c r="R3" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="36" t="s">
+      <c r="S3" s="37" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2412,10 +2412,10 @@
       <c r="O4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="36"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="37"/>
     </row>
     <row r="5" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F5" s="6" t="s">
@@ -2500,11 +2500,11 @@
     </row>
     <row r="12" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="6:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q13" s="32" t="s">
+      <c r="Q13" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
     </row>
     <row r="14" spans="6:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2536,16 +2536,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40" t="s">
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
     </row>
     <row r="3" spans="6:20" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
@@ -2625,81 +2625,81 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="42" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="E18" s="42"/>
+      <c r="G18" s="42"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="I19" s="41"/>
+      <c r="I19" s="42"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="42" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="H24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="H24" s="42"/>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="H25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="H26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="H26" s="42"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="H27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="H27" s="42"/>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="H28" s="41"/>
+      <c r="D28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="H28" s="42"/>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="H29" s="41"/>
+      <c r="D29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="H29" s="42"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
metodo para insertar documentos a nivel de bd
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C232690C-583F-42E1-AED5-6C65ECB82352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302EF2CD-C94C-4E99-95F0-81F8B84B50F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
@@ -562,7 +562,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,6 +654,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -713,7 +719,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -810,6 +816,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1396,7 +1405,7 @@
   <dimension ref="B2:L82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1553,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="32" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1600,7 +1609,7 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="43" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1716,7 +1725,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="32" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1793,7 +1802,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="43" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="2" t="s">

</xml_diff>

<commit_message>
se agrega foro, aun no se sube correcciones de las obs
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB680AF4-5E77-4159-84D5-C6B008CBFF22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4571D09C-5DEF-41D1-A3D0-3D9032235D0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
@@ -1395,7 +1395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422FE6B-CB5A-4468-BBA6-820503F36902}">
   <dimension ref="B2:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1672,7 +1672,7 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="32" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="2" t="s">

</xml_diff>

<commit_message>
Se sube la primera version de notas sin servicios
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4571D09C-5DEF-41D1-A3D0-3D9032235D0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B177FB2-D861-4AFC-9812-4B8275182820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="154">
   <si>
     <t>Trabajo</t>
   </si>
@@ -482,6 +482,24 @@
   </si>
   <si>
     <t>Fecha de inicio 20/12/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20/12/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/12/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22/12/2020</t>
+  </si>
+  <si>
+    <t>Entregado</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
   </si>
 </sst>
 </file>
@@ -562,7 +580,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,6 +672,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -713,7 +743,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -781,6 +811,9 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -811,6 +844,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1182,12 +1219,12 @@
   <dimension ref="A4:AD18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1210,6 +1247,9 @@
       <c r="E5">
         <v>30</v>
       </c>
+      <c r="F5" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1225,6 +1265,9 @@
       <c r="E6">
         <v>120</v>
       </c>
+      <c r="F6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -1240,6 +1283,9 @@
       <c r="E7">
         <v>240</v>
       </c>
+      <c r="F7" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -1255,6 +1301,9 @@
       <c r="E8">
         <v>360</v>
       </c>
+      <c r="F8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -1270,6 +1319,12 @@
       <c r="E9">
         <v>30</v>
       </c>
+      <c r="F9" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
@@ -1284,6 +1339,12 @@
       </c>
       <c r="E10" s="14">
         <v>3210</v>
+      </c>
+      <c r="F10" s="33">
+        <v>44200</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -1339,6 +1400,12 @@
       <c r="E12" s="14">
         <v>990</v>
       </c>
+      <c r="F12" s="35">
+        <v>44205</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
@@ -1353,6 +1420,12 @@
       </c>
       <c r="E13" s="15">
         <v>1890</v>
+      </c>
+      <c r="F13" s="35">
+        <v>44213</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -1395,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422FE6B-CB5A-4468-BBA6-820503F36902}">
   <dimension ref="B2:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,7 +1628,7 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="32" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1683,7 +1756,7 @@
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="32" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1804,7 +1877,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="32" t="s">
         <v>51</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1987,14 +2060,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
+    <row r="51" spans="2:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="46" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2020,14 +2093,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
+    <row r="54" spans="2:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="46" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2053,14 +2126,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
+    <row r="57" spans="2:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="46" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2342,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036ED907-70B5-4584-9CA2-BB67995731BE}">
   <dimension ref="F3:S14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="P3:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,31 +2426,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="35" t="s">
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="36" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="38" t="s">
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="38" t="s">
+      <c r="Q3" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="R3" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="37" t="s">
+      <c r="S3" s="40" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2412,10 +2485,10 @@
       <c r="O4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="37"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="40"/>
     </row>
     <row r="5" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F5" s="6" t="s">
@@ -2500,11 +2573,11 @@
     </row>
     <row r="12" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="6:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q13" s="33" t="s">
+      <c r="Q13" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="33"/>
-      <c r="S13" s="33"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
     </row>
     <row r="14" spans="6:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2536,16 +2609,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41" t="s">
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
     </row>
     <row r="3" spans="6:20" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
@@ -2625,81 +2698,81 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="45" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="42"/>
-      <c r="G18" s="42"/>
+      <c r="E18" s="45"/>
+      <c r="G18" s="45"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="I19" s="42"/>
+      <c r="I19" s="45"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="42" t="s">
+      <c r="F23" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="45" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="H24" s="42"/>
+      <c r="D24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="H24" s="45"/>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="H25" s="42"/>
+      <c r="D25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="H25" s="45"/>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="H26" s="42"/>
+      <c r="D26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="H26" s="45"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="H27" s="42"/>
+      <c r="D27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="H27" s="45"/>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="H28" s="42"/>
+      <c r="D28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="H28" s="45"/>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="H29" s="42"/>
+      <c r="D29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="H29" s="45"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Se agregan cambios de notas y avisos
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B177FB2-D861-4AFC-9812-4B8275182820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49EA7C3-4EFC-4E33-AA2B-DF64AF04896E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -814,6 +814,10 @@
     <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -844,10 +848,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422FE6B-CB5A-4468-BBA6-820503F36902}">
   <dimension ref="B2:L82"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,7 +1645,7 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="32" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1659,7 +1659,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="32" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1767,7 +1767,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="32" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="32" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1855,7 +1855,7 @@
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="32" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -1888,7 +1888,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="32" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -2060,14 +2060,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="2:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="46" t="s">
+    <row r="51" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="46" t="s">
+      <c r="C51" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="46" t="s">
+      <c r="D51" s="36" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2093,14 +2093,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="2:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="46" t="s">
+    <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="46" t="s">
+      <c r="D54" s="36" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2126,14 +2126,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="2:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="46" t="s">
+    <row r="57" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C57" s="46" t="s">
+      <c r="C57" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D57" s="46" t="s">
+      <c r="D57" s="36" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2415,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036ED907-70B5-4584-9CA2-BB67995731BE}">
   <dimension ref="F3:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="P3:S7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2426,31 +2426,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38" t="s">
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="39" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="41" t="s">
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="41" t="s">
+      <c r="Q3" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="41" t="s">
+      <c r="R3" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" s="42" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2485,10 +2485,10 @@
       <c r="O4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="40"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="42"/>
     </row>
     <row r="5" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F5" s="6" t="s">
@@ -2573,11 +2573,11 @@
     </row>
     <row r="12" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="6:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q13" s="36" t="s">
+      <c r="Q13" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
     </row>
     <row r="14" spans="6:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2609,16 +2609,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="6:20" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
@@ -2698,81 +2698,81 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="47" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="45"/>
-      <c r="G18" s="45"/>
+      <c r="E18" s="47"/>
+      <c r="G18" s="47"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="45" t="s">
+      <c r="H19" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="I19" s="45"/>
+      <c r="I19" s="47"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="45" t="s">
+      <c r="D23" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="45" t="s">
+      <c r="F23" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="H23" s="45" t="s">
+      <c r="H23" s="47" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="H24" s="45"/>
+      <c r="D24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="H24" s="47"/>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="H25" s="45"/>
+      <c r="D25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="H25" s="47"/>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="H26" s="45"/>
+      <c r="D26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="H26" s="47"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="H27" s="45"/>
+      <c r="D27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="H27" s="47"/>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="H28" s="45"/>
+      <c r="D28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="H28" s="47"/>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="H29" s="45"/>
+      <c r="D29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="H29" s="47"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
se sube todos los cambios hasta la fecha incluyendo modulo 2
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49EA7C3-4EFC-4E33-AA2B-DF64AF04896E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FAA92C-C0FC-40E2-9AD3-1F65037B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="156">
   <si>
     <t>Trabajo</t>
   </si>
@@ -500,6 +500,12 @@
   </si>
   <si>
     <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMBIOS DE ALCANCE </t>
+  </si>
+  <si>
+    <t>SEGEMENTAR SEMANAS POR MES - SEMANA</t>
   </si>
 </sst>
 </file>
@@ -580,7 +586,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,6 +690,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -743,7 +761,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -818,6 +836,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1216,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F832728-0D0A-4016-B1EB-6B174C9DD2A3}">
-  <dimension ref="A4:AD18"/>
+  <dimension ref="A4:AD21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,9 +1475,26 @@
         <v>6700</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="38">
+        <f xml:space="preserve"> 30*4</f>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1468,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422FE6B-CB5A-4468-BBA6-820503F36902}">
   <dimension ref="B2:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,7 +2100,7 @@
       </c>
     </row>
     <row r="51" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="32" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="36" t="s">
@@ -2072,7 +2111,7 @@
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="32" t="s">
         <v>67</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -2105,7 +2144,7 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="32" t="s">
         <v>69</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -2138,7 +2177,7 @@
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="32" t="s">
         <v>71</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -2191,7 +2230,7 @@
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="32" t="s">
         <v>76</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -2279,7 +2318,7 @@
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="39" t="s">
         <v>85</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -2426,31 +2465,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="40" t="s">
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="41" t="s">
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="43" t="s">
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="43" t="s">
+      <c r="R3" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="42" t="s">
+      <c r="S3" s="44" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2485,10 +2524,10 @@
       <c r="O4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="42"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="44"/>
     </row>
     <row r="5" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F5" s="6" t="s">
@@ -2573,11 +2612,11 @@
     </row>
     <row r="12" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="6:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q13" s="38" t="s">
+      <c r="Q13" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
     </row>
     <row r="14" spans="6:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2609,16 +2648,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="46" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
     </row>
     <row r="3" spans="6:20" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
@@ -2698,81 +2737,81 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="G17" s="47" t="s">
+      <c r="G17" s="49" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="E18" s="49"/>
+      <c r="G18" s="49"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="I19" s="47"/>
+      <c r="I19" s="49"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="47" t="s">
+      <c r="F23" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="H23" s="47" t="s">
+      <c r="H23" s="49" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="H24" s="47"/>
+      <c r="D24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="H24" s="49"/>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="H25" s="47"/>
+      <c r="D25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="H25" s="49"/>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="H26" s="47"/>
+      <c r="D26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="H26" s="49"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="H27" s="47"/>
+      <c r="D27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="H27" s="49"/>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="H28" s="47"/>
+      <c r="D28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="H28" s="49"/>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="H29" s="47"/>
+      <c r="D29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="H29" s="49"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
se suben los cambios para el director + docente
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FAA92C-C0FC-40E2-9AD3-1F65037B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703BF837-E923-47E4-84DB-79C9B71683D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="154">
   <si>
     <t>Trabajo</t>
   </si>
@@ -418,9 +418,6 @@
     <t>GUARDAR</t>
   </si>
   <si>
-    <t>TIEMPO DE CLASE:</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -494,9 +491,6 @@
   </si>
   <si>
     <t>Entregado</t>
-  </si>
-  <si>
-    <t>En proceso</t>
   </si>
   <si>
     <t>PENDIENTE</t>
@@ -512,7 +506,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,8 +579,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,12 +682,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -761,7 +757,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -829,15 +825,13 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4" applyAlignment="1">
@@ -869,6 +863,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1241,7 +1240,7 @@
   <dimension ref="A4:AD21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1269,7 @@
         <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -1288,7 +1287,7 @@
         <v>120</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -1306,7 +1305,7 @@
         <v>240</v>
       </c>
       <c r="F7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -1324,7 +1323,7 @@
         <v>360</v>
       </c>
       <c r="F8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -1342,10 +1341,13 @@
         <v>30</v>
       </c>
       <c r="F9" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="G9" t="s">
-        <v>151</v>
+      <c r="H9">
+        <v>6700</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -1362,11 +1364,17 @@
       <c r="E10" s="14">
         <v>3210</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="48">
         <v>44200</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>152</v>
+      <c r="G10" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="50">
+        <v>1500</v>
+      </c>
+      <c r="I10">
+        <v>6700</v>
       </c>
     </row>
     <row r="11" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -1422,11 +1430,11 @@
       <c r="E12" s="14">
         <v>990</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="48">
         <v>44205</v>
       </c>
-      <c r="G12" s="28" t="s">
-        <v>153</v>
+      <c r="G12" s="49" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -1443,11 +1451,11 @@
       <c r="E13" s="15">
         <v>1890</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="33">
         <v>44213</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -1463,6 +1471,10 @@
         <f>SUM(E6:E13)</f>
         <v>7920</v>
       </c>
+      <c r="H14">
+        <f>H9-H10-H11-H12</f>
+        <v>5200</v>
+      </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D15">
@@ -1477,22 +1489,22 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="38" t="s">
+      <c r="B21" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="35">
         <f xml:space="preserve"> 30*4</f>
         <v>120</v>
       </c>
@@ -1505,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422FE6B-CB5A-4468-BBA6-820503F36902}">
-  <dimension ref="B2:L82"/>
+  <dimension ref="A2:P82"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1689,7 @@
         <v>22</v>
       </c>
       <c r="I13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L13">
         <v>8</v>
@@ -1694,7 +1706,7 @@
         <v>22</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -1708,7 +1720,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -1722,12 +1734,12 @@
         <v>22</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1755,7 +1767,7 @@
         <v>22</v>
       </c>
       <c r="I19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L19">
         <v>8</v>
@@ -1994,7 +2006,7 @@
     </row>
     <row r="41" spans="2:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>4</v>
@@ -2025,14 +2037,14 @@
     </row>
     <row r="44" spans="2:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>55</v>
       </c>
       <c r="D44" s="26"/>
       <c r="G44" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -2070,14 +2082,14 @@
     </row>
     <row r="48" spans="2:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="18"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>16</v>
       </c>
@@ -2088,7 +2100,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>24</v>
       </c>
@@ -2099,96 +2111,200 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
       <c r="B51" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="36" t="s">
+      <c r="C51" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D51" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="21"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
       <c r="B52" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="21"/>
+      <c r="P52" s="21"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
       <c r="B53" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="37" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="36" t="s">
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="21"/>
+      <c r="O53" s="21"/>
+      <c r="P53" s="21"/>
+    </row>
+    <row r="54" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D54" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="21"/>
+      <c r="P54" s="21"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
       <c r="B55" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
+      <c r="M55" s="21"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="21"/>
+      <c r="P55" s="21"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
       <c r="B56" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="36" t="s">
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
+      <c r="P56" s="21"/>
+    </row>
+    <row r="57" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+      <c r="B57" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C57" s="36" t="s">
+      <c r="C57" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D57" s="36" t="s">
+      <c r="D57" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="21"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
       <c r="B58" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="20" t="s">
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="21"/>
+      <c r="N58" s="21"/>
+      <c r="O58" s="21"/>
+      <c r="P58" s="21"/>
+    </row>
+    <row r="59" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="32" t="s">
         <v>53</v>
       </c>
       <c r="C59" s="20" t="s">
@@ -2198,16 +2314,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="18"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>17</v>
       </c>
@@ -2218,7 +2334,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>24</v>
       </c>
@@ -2229,7 +2345,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B63" s="32" t="s">
         <v>76</v>
       </c>
@@ -2240,7 +2356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>77</v>
       </c>
@@ -2318,7 +2434,7 @@
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="39" t="s">
+      <c r="B71" s="36" t="s">
         <v>85</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -2341,7 +2457,7 @@
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>66</v>
@@ -2429,7 +2545,7 @@
     </row>
     <row r="81" spans="2:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C81" s="18" t="s">
         <v>4</v>
@@ -2438,7 +2554,7 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C82" s="17">
         <v>4</v>
@@ -2465,31 +2581,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42" t="s">
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="43" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="45" t="s">
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="45" t="s">
+      <c r="Q3" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="45" t="s">
+      <c r="R3" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="44" t="s">
+      <c r="S3" s="42" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2524,10 +2640,10 @@
       <c r="O4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="44"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="42"/>
     </row>
     <row r="5" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F5" s="6" t="s">
@@ -2612,11 +2728,11 @@
     </row>
     <row r="12" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="6:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q13" s="40" t="s">
+      <c r="Q13" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
     </row>
     <row r="14" spans="6:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2639,7 +2755,7 @@
   <dimension ref="D2:T32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,24 +2764,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="48" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0.38194444444444442</v>
-      </c>
+      <c r="I3" s="11"/>
       <c r="T3" t="s">
         <v>117</v>
       </c>
@@ -2680,7 +2791,7 @@
         <v>114</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>122</v>
@@ -2703,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T6" t="s">
         <v>120</v>
@@ -2717,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="6:20" x14ac:dyDescent="0.25">
@@ -2728,7 +2839,7 @@
         <v>0.3</v>
       </c>
       <c r="I8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="6:20" x14ac:dyDescent="0.25">
@@ -2737,81 +2848,81 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="G17" s="49" t="s">
+      <c r="E17" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E18" s="47"/>
+      <c r="G18" s="47"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="I19" s="47"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="H24" s="47"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="H25" s="47"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="H26" s="47"/>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="H27" s="47"/>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="H28" s="47"/>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="H29" s="47"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="44" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="49"/>
-      <c r="G18" s="49"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="I19" s="49"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="F23" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="H23" s="49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="H24" s="49"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="H25" s="49"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="H26" s="49"/>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="H27" s="49"/>
-    </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="H28" s="49"/>
-    </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="H29" s="49"/>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-    </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2844,7 +2955,7 @@
   <sheetData>
     <row r="8" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE ADJUNTAN ULTIMOS CAMBIOS Y LOS SCRIPT ASOCIADOS
</commit_message>
<xml_diff>
--- a/documentos/Cronograma-v1.xlsx
+++ b/documentos/Cronograma-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reibin\Trabajos\Tesis-Colegio\tesis-colegio\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3797AA4B-B1F3-45C9-8093-48E857845410}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331EBFDA-0CA2-423C-A3E1-77EB81139DCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47A00661-3571-4181-A3BA-4AB20729DD3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -757,7 +757,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -825,7 +825,6 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -836,9 +835,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1239,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F832728-0D0A-4016-B1EB-6B174C9DD2A3}">
   <dimension ref="A4:AD21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,13 +1360,13 @@
       <c r="E10" s="14">
         <v>3210</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="37">
         <v>44200</v>
       </c>
       <c r="G10" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10">
         <v>1500</v>
       </c>
       <c r="I10">
@@ -1432,10 +1428,10 @@
       <c r="E12" s="14">
         <v>990</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="37">
         <v>44205</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="38" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1453,10 +1449,10 @@
       <c r="E13" s="15">
         <v>1890</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="37">
         <v>44213</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="38" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1500,13 +1496,13 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="34">
         <f xml:space="preserve"> 30*4</f>
         <v>120</v>
       </c>
@@ -1521,7 +1517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422FE6B-CB5A-4468-BBA6-820503F36902}">
   <dimension ref="A2:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
@@ -2113,7 +2109,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="32" t="s">
         <v>65</v>
@@ -2166,10 +2162,10 @@
       <c r="B53" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="37" t="s">
+      <c r="C53" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="37" t="s">
+      <c r="D53" s="36" t="s">
         <v>56</v>
       </c>
       <c r="E53" s="21"/>
@@ -2185,7 +2181,7 @@
       <c r="O53" s="21"/>
       <c r="P53" s="21"/>
     </row>
-    <row r="54" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="32" t="s">
         <v>68</v>
@@ -2238,10 +2234,10 @@
       <c r="B56" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="37" t="s">
+      <c r="C56" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D56" s="37" t="s">
+      <c r="D56" s="36" t="s">
         <v>64</v>
       </c>
       <c r="E56" s="21"/>
@@ -2257,7 +2253,7 @@
       <c r="O56" s="21"/>
       <c r="P56" s="21"/>
     </row>
-    <row r="57" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="32" t="s">
         <v>70</v>
@@ -2436,7 +2432,7 @@
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="36" t="s">
+      <c r="B71" s="35" t="s">
         <v>85</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -2583,31 +2579,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="44" t="s">
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="46" t="s">
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="Q3" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="R3" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="45" t="s">
+      <c r="S3" s="43" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2642,10 +2638,10 @@
       <c r="O4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="45"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="43"/>
     </row>
     <row r="5" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F5" s="6" t="s">
@@ -2730,11 +2726,11 @@
     </row>
     <row r="12" spans="6:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="6:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q13" s="41" t="s">
+      <c r="Q13" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
     </row>
     <row r="14" spans="6:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2766,16 +2762,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="49" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
     </row>
     <row r="3" spans="6:20" x14ac:dyDescent="0.25">
       <c r="I3" s="11"/>
@@ -2850,81 +2846,81 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="G17" s="48" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="50"/>
-      <c r="G18" s="50"/>
+      <c r="E18" s="48"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="50"/>
+      <c r="I19" s="48"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="50" t="s">
+      <c r="D23" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="50" t="s">
+      <c r="F23" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="H23" s="50" t="s">
+      <c r="H23" s="48" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="H24" s="50"/>
+      <c r="D24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="H24" s="48"/>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="H25" s="50"/>
+      <c r="D25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="H26" s="50"/>
+      <c r="D26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="H26" s="48"/>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="H27" s="50"/>
+      <c r="D27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="H27" s="48"/>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="H28" s="50"/>
+      <c r="D28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="H28" s="48"/>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="H29" s="50"/>
+      <c r="D29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="H29" s="48"/>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="47" t="s">
+      <c r="D32" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>